<commit_message>
Update .gitignore to exclude temporary Excel files and add phase1-A: data counts frames
</commit_message>
<xml_diff>
--- a/data/public_data_resultsL.xlsx
+++ b/data/public_data_resultsL.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10817"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matusstanko/5-semester/sec-and-privacy/FinalProject/Group meow Dataset L-20251102/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matusstanko/5-semester/sec-and-privacy/sec-and-privacy-finalProject/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{721B8BD7-F24E-C64F-94BE-874B4A50FA18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18B8EE8F-0F27-4843-8893-A795B8263EE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="18600" windowHeight="18280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,9 +22,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
-    <t/>
-  </si>
-  <si>
     <t>Red</t>
   </si>
   <si>
@@ -50,6 +47,9 @@
   </si>
   <si>
     <t>E-votes</t>
+  </si>
+  <si>
+    <t>party</t>
   </si>
 </sst>
 </file>
@@ -385,7 +385,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
@@ -394,24 +396,24 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
-      </c>
-      <c r="E1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2">
         <v>26</v>
@@ -428,7 +430,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B3">
         <v>67</v>
@@ -445,7 +447,7 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4">
         <v>96</v>
@@ -462,7 +464,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B5">
         <v>89</v>
@@ -479,7 +481,7 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B6">
         <v>130</v>
@@ -496,7 +498,7 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B7">
         <v>408</v>
@@ -518,12 +520,14 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7f72b764-4b0f-4352-b2a3-29d337326309">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="0ddf43ae-6642-4ea9-b706-07519d4cc3e0" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -722,20 +726,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="7f72b764-4b0f-4352-b2a3-29d337326309">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="0ddf43ae-6642-4ea9-b706-07519d4cc3e0" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{79EB9EDA-280B-4E8E-8F6B-520A7E0E0A66}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5CAA431-FCB4-44E8-AC55-80F973A7F2D2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="7f72b764-4b0f-4352-b2a3-29d337326309"/>
+    <ds:schemaRef ds:uri="0ddf43ae-6642-4ea9-b706-07519d4cc3e0"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -760,12 +765,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5CAA431-FCB4-44E8-AC55-80F973A7F2D2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{79EB9EDA-280B-4E8E-8F6B-520A7E0E0A66}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="7f72b764-4b0f-4352-b2a3-29d337326309"/>
-    <ds:schemaRef ds:uri="0ddf43ae-6642-4ea9-b706-07519d4cc3e0"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Refactor phase1-A notebook: update data loading, enhance markdown sections, and correct column names for clarity
</commit_message>
<xml_diff>
--- a/data/public_data_resultsL.xlsx
+++ b/data/public_data_resultsL.xlsx
@@ -8,19 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/matusstanko/5-semester/sec-and-privacy/sec-and-privacy-finalProject/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18B8EE8F-0F27-4843-8893-A795B8263EE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CAD49B2B-D755-FC4D-B2A6-24AB0E8B541D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="18600" windowHeight="18280" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet 1" sheetId="1" r:id="rId1"/>
+    <sheet name="pivot" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet 1" sheetId="1" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="11">
   <si>
     <t>Red</t>
   </si>
@@ -50,6 +64,9 @@
   </si>
   <si>
     <t>party</t>
+  </si>
+  <si>
+    <t>Offline-votes</t>
   </si>
 </sst>
 </file>
@@ -382,11 +399,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A520727-EF8B-4B45-847A-4BC91969E9DA}">
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -413,6 +430,94 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>278</v>
+      </c>
+      <c r="C2">
+        <v>406</v>
+      </c>
+      <c r="D2">
+        <v>18</v>
+      </c>
+      <c r="E2">
+        <f>SUM(B2:D2)</f>
+        <v>702</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3">
+        <v>130</v>
+      </c>
+      <c r="C3">
+        <v>206</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>337</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4">
+        <v>408</v>
+      </c>
+      <c r="C4">
+        <v>612</v>
+      </c>
+      <c r="D4">
+        <v>19</v>
+      </c>
+      <c r="E4">
+        <v>1039</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="35.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
       <c r="B2">
@@ -531,6 +636,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100EFF4F8DD4AF95548A29E5B36B9FF92C8" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="ab34acb651412efa50d0579d77d1b472">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7f72b764-4b0f-4352-b2a3-29d337326309" xmlns:ns3="0ddf43ae-6642-4ea9-b706-07519d4cc3e0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="1609f74860d2836c40a0786265c30a43" ns2:_="" ns3:_="">
     <xsd:import namespace="7f72b764-4b0f-4352-b2a3-29d337326309"/>
@@ -725,15 +839,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5CAA431-FCB4-44E8-AC55-80F973A7F2D2}">
   <ds:schemaRefs>
@@ -746,6 +851,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{79EB9EDA-280B-4E8E-8F6B-520A7E0E0A66}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{316971CD-810D-4040-9379-9516E36B26A5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -762,12 +875,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{79EB9EDA-280B-4E8E-8F6B-520A7E0E0A66}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>